<commit_message>
chore: cleaned excel report for classifier performance
</commit_message>
<xml_diff>
--- a/classification_report.xlsx
+++ b/classification_report.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user_\Desktop\NLP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user_\Desktop\NLP\NLP-GENIUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15CF804A-33B8-47E1-B095-9BE4FDC5BE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F82714-21B0-4568-8417-DC96EFEBAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Au propre" sheetId="2" r:id="rId1"/>
+    <sheet name="Raw data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="69">
   <si>
     <t>precision</t>
   </si>
@@ -274,6 +275,135 @@
   </si>
   <si>
     <t>scoring = 'accuracy'</t>
+  </si>
+  <si>
+    <t>acuracy</t>
+  </si>
+  <si>
+    <t>temps</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Résultat cumulé</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>macro-avg</t>
+  </si>
+  <si>
+    <t>weighted-avg</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">df = pd.read_csv("song_lyrics.csv", skiprows=lambda i: i % </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> != 0)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>df = pd.read_csv("song_lyrics.csv", skiprows=lambda i: i %</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 10 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>!= 0)</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt;60</t>
+  </si>
+  <si>
+    <t>Nombre de cv=3</t>
+  </si>
+  <si>
+    <t>Best penalty found : l2</t>
+  </si>
+  <si>
+    <t>Best C found : 0,01</t>
+  </si>
+  <si>
+    <t>On prend 1 /100 des données</t>
+  </si>
+  <si>
+    <t>On prend 1 /10 des données</t>
+  </si>
+  <si>
+    <t>On prend 1 /10 des données et on performe une Cross Validation</t>
+  </si>
+  <si>
+    <t>Avec Grid Search</t>
+  </si>
+  <si>
+    <r>
+      <t>scores = cross_val_score(model, X, Y,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cv=5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, scoring=scoring, n_jobs = -1)</t>
+    </r>
+  </si>
+  <si>
+    <t>Avec un ensembling</t>
+  </si>
+  <si>
+    <t>temps d'éxécution en min</t>
   </si>
 </sst>
 </file>
@@ -302,7 +432,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +466,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -393,6 +541,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,16 +567,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>370718</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>94679</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>5609468</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>151829</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -446,7 +599,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16182975" y="6762750"/>
+          <a:off x="14268450" y="10058400"/>
           <a:ext cx="6057143" cy="4571429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -743,19 +896,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C91141-D424-4D2B-9584-7FFDD620E3BC}">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="116" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>0.64</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>0.39</v>
+      </c>
+      <c r="E3" s="10">
+        <v>0.62165109034267918</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0.59</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.35</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.59922118380062306</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0.38</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.60950155763239877</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0.65</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.42159620955825122</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.65615912887459016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0.65</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.422485899</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.65634473800000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32">
+        <v>0.65</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="121.140625" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" customWidth="1"/>
-    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="110.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chore: last edit on classifier, going on main to merge
</commit_message>
<xml_diff>
--- a/classification_report.xlsx
+++ b/classification_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user_\Desktop\NLP\NLP-GENIUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F82714-21B0-4568-8417-DC96EFEBAD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF22FC53-A31A-4623-A726-6BEE8C9E062E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3585" yWindow="3000" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Au propre" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="75">
   <si>
     <t>precision</t>
   </si>
@@ -280,21 +280,6 @@
     <t>acuracy</t>
   </si>
   <si>
-    <t>temps</t>
-  </si>
-  <si>
-    <t>Somme</t>
-  </si>
-  <si>
-    <t>Moyenne</t>
-  </si>
-  <si>
-    <t>Résultat cumulé</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>macro-avg</t>
   </si>
   <si>
@@ -404,13 +389,618 @@
   </si>
   <si>
     <t>temps d'éxécution en min</t>
+  </si>
+  <si>
+    <t>naive_bayes (multinomial NB)</t>
+  </si>
+  <si>
+    <r>
+      <t>model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF795E26"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>make_pipeline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF267F99"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CountVectorizer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ngram_range</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF267F99"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MultinomialNB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>alpha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>pipeline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF267F99"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Pipeline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>([</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vectorizer'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF267F99"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>CountVectorizer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>tokenizer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF795E26"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>gpt_tokenize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>stop_words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF267F99"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>en_stop</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))),</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'classifier'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF267F99"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>MultinomialNB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>force_alpha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>True</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>))</t>
+    </r>
+  </si>
+  <si>
+    <t>    ])</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF001080"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>param_grid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> = {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'vectorizer__ngram_range'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: [(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>), (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)],</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'classifier__alpha'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF098658"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>    }</t>
+  </si>
+  <si>
+    <t>misc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,8 +1021,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF001080"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF795E26"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF267F99"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF098658"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -487,6 +1119,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -524,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -544,8 +1182,16 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C91141-D424-4D2B-9584-7FFDD620E3BC}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -912,24 +1558,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -984,20 +1630,20 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1008,7 +1654,7 @@
         <v>0.65</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="10">
         <v>0.42159620955825122</v>
@@ -1025,7 +1671,7 @@
         <v>0.65</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D10" s="10">
         <v>0.422485899</v>
@@ -1035,22 +1681,21 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="13"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1062,7 +1707,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,7 +1715,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,7 +1730,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,33 +1749,30 @@
         <v>37</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1149,13 +1791,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B32">
         <v>0.65</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1165,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G108"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,7 +2756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>34</v>
       </c>
@@ -2122,27 +2764,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>47</v>
       </c>
@@ -2150,9 +2792,256 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B112" t="s">
+        <v>0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1</v>
+      </c>
+      <c r="D112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B113">
+        <v>0.1</v>
+      </c>
+      <c r="C113">
+        <v>0.01</v>
+      </c>
+      <c r="D113">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>74</v>
+      </c>
+      <c r="B114">
+        <v>0.48</v>
+      </c>
+      <c r="C114">
+        <v>0.61</v>
+      </c>
+      <c r="D114">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C115">
+        <v>0.69</v>
+      </c>
+      <c r="D115">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116">
+        <v>0.81</v>
+      </c>
+      <c r="C116">
+        <v>0.81</v>
+      </c>
+      <c r="D116">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117">
+        <v>0.25</v>
+      </c>
+      <c r="C117">
+        <v>0.05</v>
+      </c>
+      <c r="D117">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118">
+        <v>0.43</v>
+      </c>
+      <c r="C118">
+        <v>0.38</v>
+      </c>
+      <c r="D118">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>9</v>
+      </c>
+      <c r="B121" s="3">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>10</v>
+      </c>
+      <c r="B122">
+        <v>0.44</v>
+      </c>
+      <c r="C122">
+        <v>0.42</v>
+      </c>
+      <c r="D122">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>11</v>
+      </c>
+      <c r="B123">
+        <v>0.59</v>
+      </c>
+      <c r="C123">
+        <v>0.62</v>
+      </c>
+      <c r="D123">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="16"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>0</v>
+      </c>
+      <c r="C142" t="s">
+        <v>1</v>
+      </c>
+      <c r="D142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>9</v>
+      </c>
+      <c r="B151">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>10</v>
+      </c>
+      <c r="B152">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>11</v>
+      </c>
+      <c r="B153">
+        <v>0.57499999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>